<commit_message>
implementacion por terminar de escritura de datos en el excel del dr Rolando
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco_elementos_inclinados.xlsx
+++ b/pruebas_excel/marco_elementos_inclinados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4A348AB-2DA9-431F-97C8-945C76D3D1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673A1069-A4D7-4E34-AAED-4E9A8B728459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="961" activeTab="1" xr2:uid="{AEB2A8C3-3115-477C-A812-7952A4648430}"/>
+    <workbookView xWindow="28680" yWindow="1815" windowWidth="24240" windowHeight="13740" tabRatio="961" firstSheet="15" activeTab="22" xr2:uid="{AEB2A8C3-3115-477C-A812-7952A4648430}"/>
   </bookViews>
   <sheets>
     <sheet name="Assembled Joint Masses" sheetId="1" r:id="rId1"/>
@@ -4248,7 +4248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC8D54E-780D-424D-ADB0-E876363FD9FD}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -5066,9 +5066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A12D3F-D89C-46FD-9CE3-41240B07F713}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>